<commit_message>
Changes on 3rd Sept 2012
JQueryUI, Prompt, and Customer forms.
TBD: multiple database support
</commit_message>
<xml_diff>
--- a/docs/AppStart Database ver1.0.xlsx
+++ b/docs/AppStart Database ver1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="1425" yWindow="-30" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="87">
   <si>
     <t>tbl_User</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Updated By</t>
-  </si>
-  <si>
-    <t>Customer User name</t>
   </si>
   <si>
     <t>tbl_Module</t>
@@ -285,8 +282,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +337,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -418,6 +420,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -452,6 +455,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -627,14 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:AF54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:AF53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="1.28515625" customWidth="1"/>
@@ -670,16 +674,16 @@
     <col min="33" max="33" width="0.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:32">
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="s">
@@ -692,10 +696,10 @@
         <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R3" s="1"/>
       <c r="T3" s="1"/>
@@ -706,7 +710,7 @@
       <c r="AD3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="2:32">
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -733,9 +737,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:32">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>1</v>
@@ -754,10 +758,10 @@
         <v>31</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="2:32">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -768,8 +772,8 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>4</v>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="J6" t="s">
         <v>4</v>
@@ -778,15 +782,15 @@
         <v>1</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="2:32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>17</v>
@@ -795,22 +799,22 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>45</v>
+      <c r="H7" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="N7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" t="s">
         <v>11</v>
       </c>
       <c r="AD7" s="5"/>
     </row>
-    <row r="8" spans="2:32">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
@@ -822,23 +826,23 @@
         <v>26</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AD8" s="5"/>
     </row>
-    <row r="9" spans="2:32">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
@@ -851,7 +855,7 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" t="s">
         <v>25</v>
@@ -860,14 +864,14 @@
         <v>23</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="2:32">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
@@ -877,8 +881,8 @@
         <v>17</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>11</v>
+      <c r="H10" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="J10" t="s">
         <v>5</v>
@@ -890,11 +894,11 @@
         <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD10" s="5"/>
     </row>
-    <row r="11" spans="2:32">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
@@ -907,7 +911,7 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -916,14 +920,14 @@
         <v>22</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="2:32">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
@@ -932,8 +936,8 @@
         <v>19</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
-        <v>15</v>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -943,139 +947,139 @@
         <v>36</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="2:32">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="5"/>
       <c r="H13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J13" s="4"/>
       <c r="N13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Z13" s="4"/>
     </row>
-    <row r="14" spans="2:32">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="H14" s="4" t="s">
-        <v>14</v>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="J14" s="4"/>
       <c r="N14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="P14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T14" s="1"/>
       <c r="V14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Z14" s="4"/>
     </row>
-    <row r="15" spans="2:32">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="5"/>
       <c r="H15" s="5" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="J15" s="4"/>
       <c r="N15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Z15" s="4"/>
     </row>
-    <row r="16" spans="2:32">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J16" s="4"/>
       <c r="P16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Z16" s="4"/>
       <c r="AB16" s="5"/>
     </row>
-    <row r="17" spans="4:28">
+    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="4"/>
       <c r="H17" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Z17" s="4"/>
       <c r="AB17" s="5"/>
     </row>
-    <row r="18" spans="4:28">
+    <row r="18" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="H18" s="5" t="s">
-        <v>36</v>
+      <c r="H18" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Z18" s="4"/>
       <c r="AB18" s="5"/>
     </row>
-    <row r="19" spans="4:28">
+    <row r="19" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="1"/>
       <c r="P19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Z19" s="4"/>
       <c r="AB19" s="5"/>
     </row>
-    <row r="20" spans="4:28">
+    <row r="20" spans="4:28" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P20" t="s">
         <v>16</v>
@@ -1084,23 +1088,20 @@
       <c r="X20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
-    <row r="21" spans="4:28">
+    <row r="21" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="H21" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N21" s="5"/>
       <c r="P21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Z21" s="4"/>
     </row>
-    <row r="22" spans="4:28">
+    <row r="22" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
         <v>23</v>
       </c>
@@ -1113,11 +1114,14 @@
       <c r="X22" s="4"/>
       <c r="Z22" s="4"/>
     </row>
-    <row r="23" spans="4:28">
+    <row r="23" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="5"/>
+      <c r="H23" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="N23" s="5"/>
       <c r="P23" s="4" t="s">
@@ -1127,13 +1131,13 @@
       <c r="X23" s="4"/>
       <c r="Z23" s="4"/>
     </row>
-    <row r="24" spans="4:28">
+    <row r="24" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="H24" s="7" t="s">
-        <v>37</v>
+      <c r="H24" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J24" s="4"/>
       <c r="N24" s="5"/>
@@ -1144,13 +1148,13 @@
       <c r="X24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="4:28">
+    <row r="25" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="J25" s="4"/>
       <c r="P25" s="4" t="s">
@@ -1161,10 +1165,10 @@
       <c r="X25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" spans="4:28">
+    <row r="26" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E26" s="7"/>
       <c r="H26" s="5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="J26" s="4"/>
       <c r="T26" s="5"/>
@@ -1172,10 +1176,10 @@
       <c r="X26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" spans="4:28">
+    <row r="27" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J27" s="5"/>
       <c r="T27" s="5"/>
@@ -1183,48 +1187,48 @@
       <c r="X27" s="4"/>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="4:28">
+    <row r="28" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T28" s="5"/>
       <c r="V28" s="4"/>
       <c r="X28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" spans="4:28">
+    <row r="29" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V29" s="4"/>
       <c r="X29" s="4"/>
       <c r="Z29" s="4"/>
     </row>
-    <row r="30" spans="4:28">
+    <row r="30" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V30" s="4"/>
       <c r="X30" s="4"/>
       <c r="Z30" s="4"/>
     </row>
-    <row r="31" spans="4:28">
+    <row r="31" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T31" s="1"/>
       <c r="V31" s="5"/>
       <c r="X31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="4:28">
+    <row r="32" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J32" s="1"/>
       <c r="T32" s="5"/>
@@ -1232,136 +1236,129 @@
       <c r="X32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="4:26">
+    <row r="33" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="H33" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="H33" s="5"/>
       <c r="V33" s="5"/>
       <c r="X33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="4:26">
+    <row r="34" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="H34" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="V34" s="5"/>
       <c r="X34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="4:26">
+    <row r="35" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="H35" s="7" t="s">
-        <v>52</v>
+      <c r="H35" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="T35" s="5"/>
     </row>
-    <row r="36" spans="4:26">
+    <row r="36" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H36" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J36" s="5"/>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" spans="4:26">
+    <row r="37" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H37" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="J37" s="5"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="4:26">
+    <row r="38" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H38" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="J38" s="5"/>
       <c r="T38" s="5"/>
     </row>
-    <row r="39" spans="4:26">
+    <row r="39" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H39" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="4:26">
+    <row r="40" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H40" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="4:26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H41" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="4:26">
+    <row r="42" spans="4:26" x14ac:dyDescent="0.25">
       <c r="H42" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="H43" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="H45" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="H46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="H47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="4:26">
-      <c r="H43" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="4:26">
-      <c r="H44" s="5" t="s">
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R49" s="5"/>
+    </row>
+    <row r="50" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>10</v>
+      </c>
+      <c r="R50" s="5"/>
+    </row>
+    <row r="51" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H51" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="45" spans="4:26">
-      <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="4:26">
-      <c r="H46" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="4:26">
-      <c r="H47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="T47" s="5"/>
-    </row>
-    <row r="48" spans="4:26">
-      <c r="H48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T48" s="5"/>
-    </row>
-    <row r="49" spans="8:18">
-      <c r="R49" s="5"/>
-    </row>
-    <row r="50" spans="8:18">
-      <c r="H50" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R50" s="5"/>
-    </row>
-    <row r="51" spans="8:18">
-      <c r="H51" t="s">
-        <v>10</v>
-      </c>
       <c r="R51" s="5"/>
     </row>
-    <row r="52" spans="8:18">
+    <row r="52" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H52" s="5" t="s">
         <v>84</v>
       </c>
       <c r="R52" s="5"/>
     </row>
-    <row r="53" spans="8:18">
+    <row r="53" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H53" s="5" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="8:18">
-      <c r="H54" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1371,14 +1368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="1.140625" customWidth="1"/>
@@ -1392,24 +1389,24 @@
     <col min="10" max="10" width="1.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1426,9 +1423,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1437,13 +1434,13 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1454,13 +1451,13 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1474,9 +1471,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>34</v>
@@ -1486,75 +1483,75 @@
       </c>
       <c r="G7" s="5"/>
       <c r="I7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
       <c r="I8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
       <c r="I9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
       <c r="I10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="4"/>
       <c r="I11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="I12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="I13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="I14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="I15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="I16" t="s">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="9:9">
-      <c r="I17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1563,12 +1560,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>